<commit_message>
i did a little today but it doesn't matter
</commit_message>
<xml_diff>
--- a/Blopnote/blopnote bugs and notes.xlsx
+++ b/Blopnote/blopnote bugs and notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azgel\source\repos\Blopnote\Blopnote\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F97F2271-C5B2-459C-AC0A-B5EF8108C622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78CC8C86-6C57-4386-9235-D6B2CADB4E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7D1902E2-70B7-47CB-86DF-C5450FDE41FB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="75">
   <si>
     <t>ID</t>
   </si>
@@ -247,6 +247,9 @@
   </si>
   <si>
     <t>hotkeys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">const MAX_WIDTH added </t>
   </si>
 </sst>
 </file>
@@ -670,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE5A6968-05AB-409C-B696-8DB44652D9F9}">
   <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,7 +921,7 @@
       <c r="E10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
@@ -993,7 +996,10 @@
       <c r="E14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="1"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="4">

</xml_diff>

<commit_message>
tuz tuz tuz tuz
</commit_message>
<xml_diff>
--- a/Blopnote/blopnote bugs and notes.xlsx
+++ b/Blopnote/blopnote bugs and notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azgel\source\repos\Blopnote\Blopnote\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{536A8EDB-914F-4692-91D9-C981CA281A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5123000-78AC-45D1-9E6A-B0B4877C3F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7D1902E2-70B7-47CB-86DF-C5450FDE41FB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="100">
   <si>
     <t>ID</t>
   </si>
@@ -318,6 +318,18 @@
   </si>
   <si>
     <t>user can look at the song translation from google during writing of his translation by holding TAB</t>
+  </si>
+  <si>
+    <t>lyrics not found from first attempt</t>
+  </si>
+  <si>
+    <t>but ones found in other attempts</t>
+  </si>
+  <si>
+    <t>index out of range for tab</t>
+  </si>
+  <si>
+    <t>only first x translated lines displayed for n lines where x &lt; n</t>
   </si>
 </sst>
 </file>
@@ -745,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE5A6968-05AB-409C-B696-8DB44652D9F9}">
   <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1471,19 +1483,35 @@
       </c>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>36</v>
       </c>
+      <c r="B37" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E37" s="11"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>37</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
+      <c r="B38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="E38" s="3"/>
       <c r="F38" s="1"/>
     </row>
@@ -1541,36 +1569,60 @@
       <c r="A44" s="4">
         <v>43</v>
       </c>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
       <c r="F44" s="1"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>44</v>
       </c>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
       <c r="F45" s="1"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>45</v>
       </c>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
       <c r="F46" s="1"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>46</v>
       </c>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
       <c r="F47" s="1"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>47</v>
       </c>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
       <c r="F48" s="1"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>48</v>
       </c>
+      <c r="B49" s="11"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
       <c r="F49" s="1"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
i do everything and nothing
</commit_message>
<xml_diff>
--- a/Blopnote/blopnote bugs and notes.xlsx
+++ b/Blopnote/blopnote bugs and notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azgel\source\repos\Blopnote\Blopnote\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A119F34-65A6-4395-B1D9-29CFD8569237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9663807E-8F8B-4BFD-AB89-781342B4D575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7D1902E2-70B7-47CB-86DF-C5450FDE41FB}"/>
+    <workbookView xWindow="15" yWindow="0" windowWidth="28710" windowHeight="11145" xr2:uid="{7D1902E2-70B7-47CB-86DF-C5450FDE41FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="103">
   <si>
     <t>ID</t>
   </si>
@@ -336,6 +336,9 @@
   </si>
   <si>
     <t>in case when google translator didn't give results or user want to refresh translation</t>
+  </si>
+  <si>
+    <t>after dream browser is disconnected</t>
   </si>
 </sst>
 </file>
@@ -763,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE5A6968-05AB-409C-B696-8DB44652D9F9}">
   <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1537,12 +1540,16 @@
       <c r="E39" s="3"/>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>39</v>
       </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
+      <c r="B40" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="1"/>
@@ -1561,7 +1568,6 @@
       <c r="A42" s="4">
         <v>41</v>
       </c>
-      <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>

</xml_diff>

<commit_message>
browser refactoring + MessageShower. seems cute
</commit_message>
<xml_diff>
--- a/Blopnote/blopnote bugs and notes.xlsx
+++ b/Blopnote/blopnote bugs and notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azgel\source\repos\Blopnote\Blopnote\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9663807E-8F8B-4BFD-AB89-781342B4D575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC080D6C-B825-4127-A09A-4D4D737F8165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="0" windowWidth="28710" windowHeight="11145" xr2:uid="{7D1902E2-70B7-47CB-86DF-C5450FDE41FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7D1902E2-70B7-47CB-86DF-C5450FDE41FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="109">
   <si>
     <t>ID</t>
   </si>
@@ -339,6 +339,24 @@
   </si>
   <si>
     <t>after dream browser is disconnected</t>
+  </si>
+  <si>
+    <t>Application.Exit()</t>
+  </si>
+  <si>
+    <t>doesn't work</t>
+  </si>
+  <si>
+    <t>app executes code after Exit()</t>
+  </si>
+  <si>
+    <t>How to add console to winforms app</t>
+  </si>
+  <si>
+    <t>and file logging</t>
+  </si>
+  <si>
+    <t>FileProcessor.AskPath() works in awkward way</t>
   </si>
 </sst>
 </file>
@@ -420,7 +438,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -450,6 +468,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -764,16 +785,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE5A6968-05AB-409C-B696-8DB44652D9F9}">
-  <dimension ref="A1:P50"/>
+  <dimension ref="A1:P145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
     <col min="3" max="3" width="23.140625" customWidth="1"/>
     <col min="4" max="4" width="22.7109375" customWidth="1"/>
     <col min="7" max="7" width="27.85546875" customWidth="1"/>
@@ -1426,7 +1447,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -1442,7 +1463,7 @@
       </c>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -1460,7 +1481,7 @@
       </c>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -1476,7 +1497,7 @@
       </c>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -1492,7 +1513,7 @@
       </c>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -1508,7 +1529,7 @@
       <c r="E37" s="11"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -1524,7 +1545,7 @@
       <c r="E38" s="3"/>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -1538,9 +1559,10 @@
         <v>101</v>
       </c>
       <c r="E39" s="3"/>
-      <c r="F39" s="1"/>
-    </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F39" s="13"/>
+      <c r="G39" s="3"/>
+    </row>
+    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -1552,9 +1574,10 @@
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
-      <c r="F40" s="1"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F40" s="13"/>
+      <c r="G40" s="3"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -1562,89 +1585,876 @@
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
-      <c r="F41" s="1"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F41" s="13"/>
+      <c r="G41" s="3"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>41</v>
       </c>
+      <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
-      <c r="F42" s="1"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F42" s="13"/>
+      <c r="G42" s="3"/>
+    </row>
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>42</v>
       </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
+      <c r="B43" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="E43" s="3"/>
-      <c r="F43" s="1"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F43" s="13"/>
+      <c r="G43" s="3"/>
+    </row>
+    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>43</v>
       </c>
-      <c r="B44" s="11"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="1"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="3"/>
+    </row>
+    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>44</v>
       </c>
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="1"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="3"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>45</v>
       </c>
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="1"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="3"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>46</v>
       </c>
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="1"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="3"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>47</v>
       </c>
-      <c r="B48" s="11"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="1"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="3"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>48</v>
       </c>
-      <c r="B49" s="11"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="1"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="3"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
       <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3"/>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="3"/>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="3"/>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="3"/>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3"/>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3"/>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B84" s="3"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3"/>
+      <c r="G84" s="3"/>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3"/>
+      <c r="G85" s="3"/>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B86" s="3"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3"/>
+      <c r="G86" s="3"/>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
+      <c r="G87" s="3"/>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+      <c r="G88" s="3"/>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3"/>
+      <c r="G89" s="3"/>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3"/>
+      <c r="G90" s="3"/>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="3"/>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3"/>
+      <c r="G92" s="3"/>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B93" s="3"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="3"/>
+      <c r="G93" s="3"/>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B94" s="3"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="3"/>
+      <c r="G94" s="3"/>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="3"/>
+      <c r="G95" s="3"/>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="3"/>
+      <c r="G96" s="3"/>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B97" s="3"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="3"/>
+      <c r="G97" s="3"/>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B98" s="3"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="3"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="3"/>
+      <c r="G98" s="3"/>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B99" s="3"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="3"/>
+      <c r="F99" s="3"/>
+      <c r="G99" s="3"/>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B100" s="3"/>
+      <c r="C100" s="3"/>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3"/>
+      <c r="G100" s="3"/>
+    </row>
+    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B101" s="3"/>
+      <c r="C101" s="3"/>
+      <c r="D101" s="3"/>
+      <c r="E101" s="3"/>
+      <c r="F101" s="3"/>
+      <c r="G101" s="3"/>
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B102" s="3"/>
+      <c r="C102" s="3"/>
+      <c r="D102" s="3"/>
+      <c r="E102" s="3"/>
+      <c r="F102" s="3"/>
+      <c r="G102" s="3"/>
+    </row>
+    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B103" s="3"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
+      <c r="E103" s="3"/>
+      <c r="F103" s="3"/>
+      <c r="G103" s="3"/>
+    </row>
+    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B104" s="3"/>
+      <c r="C104" s="3"/>
+      <c r="D104" s="3"/>
+      <c r="E104" s="3"/>
+      <c r="F104" s="3"/>
+      <c r="G104" s="3"/>
+    </row>
+    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B105" s="3"/>
+      <c r="C105" s="3"/>
+      <c r="D105" s="3"/>
+      <c r="E105" s="3"/>
+      <c r="F105" s="3"/>
+      <c r="G105" s="3"/>
+    </row>
+    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B106" s="3"/>
+      <c r="C106" s="3"/>
+      <c r="D106" s="3"/>
+      <c r="E106" s="3"/>
+      <c r="F106" s="3"/>
+      <c r="G106" s="3"/>
+    </row>
+    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B107" s="3"/>
+      <c r="C107" s="3"/>
+      <c r="D107" s="3"/>
+      <c r="E107" s="3"/>
+      <c r="F107" s="3"/>
+      <c r="G107" s="3"/>
+    </row>
+    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B108" s="3"/>
+      <c r="C108" s="3"/>
+      <c r="D108" s="3"/>
+      <c r="E108" s="3"/>
+      <c r="F108" s="3"/>
+      <c r="G108" s="3"/>
+    </row>
+    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B109" s="3"/>
+      <c r="C109" s="3"/>
+      <c r="D109" s="3"/>
+      <c r="E109" s="3"/>
+      <c r="F109" s="3"/>
+      <c r="G109" s="3"/>
+    </row>
+    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B110" s="3"/>
+      <c r="C110" s="3"/>
+      <c r="D110" s="3"/>
+      <c r="E110" s="3"/>
+      <c r="F110" s="3"/>
+      <c r="G110" s="3"/>
+    </row>
+    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B111" s="3"/>
+      <c r="C111" s="3"/>
+      <c r="D111" s="3"/>
+      <c r="E111" s="3"/>
+      <c r="F111" s="3"/>
+      <c r="G111" s="3"/>
+    </row>
+    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B112" s="3"/>
+      <c r="C112" s="3"/>
+      <c r="D112" s="3"/>
+      <c r="E112" s="3"/>
+      <c r="F112" s="3"/>
+      <c r="G112" s="3"/>
+    </row>
+    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B113" s="3"/>
+      <c r="C113" s="3"/>
+      <c r="D113" s="3"/>
+      <c r="E113" s="3"/>
+      <c r="F113" s="3"/>
+      <c r="G113" s="3"/>
+    </row>
+    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B114" s="3"/>
+      <c r="C114" s="3"/>
+      <c r="D114" s="3"/>
+      <c r="E114" s="3"/>
+      <c r="F114" s="3"/>
+      <c r="G114" s="3"/>
+    </row>
+    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B115" s="3"/>
+      <c r="C115" s="3"/>
+      <c r="D115" s="3"/>
+      <c r="E115" s="3"/>
+      <c r="F115" s="3"/>
+      <c r="G115" s="3"/>
+    </row>
+    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B116" s="3"/>
+      <c r="C116" s="3"/>
+      <c r="D116" s="3"/>
+      <c r="E116" s="3"/>
+      <c r="F116" s="3"/>
+      <c r="G116" s="3"/>
+    </row>
+    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B117" s="3"/>
+      <c r="C117" s="3"/>
+      <c r="D117" s="3"/>
+      <c r="E117" s="3"/>
+      <c r="F117" s="3"/>
+      <c r="G117" s="3"/>
+    </row>
+    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B118" s="3"/>
+      <c r="C118" s="3"/>
+      <c r="D118" s="3"/>
+      <c r="E118" s="3"/>
+      <c r="F118" s="3"/>
+      <c r="G118" s="3"/>
+    </row>
+    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B119" s="3"/>
+      <c r="C119" s="3"/>
+      <c r="D119" s="3"/>
+      <c r="E119" s="3"/>
+      <c r="F119" s="3"/>
+      <c r="G119" s="3"/>
+    </row>
+    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B120" s="3"/>
+      <c r="C120" s="3"/>
+      <c r="D120" s="3"/>
+      <c r="E120" s="3"/>
+      <c r="F120" s="3"/>
+      <c r="G120" s="3"/>
+    </row>
+    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B121" s="3"/>
+      <c r="C121" s="3"/>
+      <c r="D121" s="3"/>
+      <c r="E121" s="3"/>
+      <c r="F121" s="3"/>
+      <c r="G121" s="3"/>
+    </row>
+    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B122" s="3"/>
+      <c r="C122" s="3"/>
+      <c r="D122" s="3"/>
+      <c r="E122" s="3"/>
+      <c r="F122" s="3"/>
+      <c r="G122" s="3"/>
+    </row>
+    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B123" s="3"/>
+      <c r="C123" s="3"/>
+      <c r="D123" s="3"/>
+      <c r="E123" s="3"/>
+      <c r="F123" s="3"/>
+      <c r="G123" s="3"/>
+    </row>
+    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B124" s="3"/>
+      <c r="C124" s="3"/>
+      <c r="D124" s="3"/>
+      <c r="E124" s="3"/>
+      <c r="F124" s="3"/>
+      <c r="G124" s="3"/>
+    </row>
+    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B125" s="3"/>
+      <c r="C125" s="3"/>
+      <c r="D125" s="3"/>
+      <c r="E125" s="3"/>
+      <c r="F125" s="3"/>
+      <c r="G125" s="3"/>
+    </row>
+    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B126" s="3"/>
+      <c r="C126" s="3"/>
+      <c r="D126" s="3"/>
+      <c r="E126" s="3"/>
+      <c r="F126" s="3"/>
+      <c r="G126" s="3"/>
+    </row>
+    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B127" s="3"/>
+      <c r="C127" s="3"/>
+      <c r="D127" s="3"/>
+      <c r="E127" s="3"/>
+      <c r="F127" s="3"/>
+      <c r="G127" s="3"/>
+    </row>
+    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B128" s="3"/>
+      <c r="C128" s="3"/>
+      <c r="D128" s="3"/>
+      <c r="E128" s="3"/>
+      <c r="F128" s="3"/>
+      <c r="G128" s="3"/>
+    </row>
+    <row r="129" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B129" s="3"/>
+      <c r="C129" s="3"/>
+      <c r="D129" s="3"/>
+      <c r="E129" s="3"/>
+      <c r="F129" s="3"/>
+      <c r="G129" s="3"/>
+    </row>
+    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B130" s="3"/>
+      <c r="C130" s="3"/>
+      <c r="D130" s="3"/>
+      <c r="E130" s="3"/>
+      <c r="F130" s="3"/>
+      <c r="G130" s="3"/>
+    </row>
+    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B131" s="3"/>
+      <c r="C131" s="3"/>
+      <c r="D131" s="3"/>
+      <c r="E131" s="3"/>
+      <c r="F131" s="3"/>
+      <c r="G131" s="3"/>
+    </row>
+    <row r="132" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B132" s="3"/>
+      <c r="C132" s="3"/>
+      <c r="D132" s="3"/>
+      <c r="E132" s="3"/>
+      <c r="F132" s="3"/>
+      <c r="G132" s="3"/>
+    </row>
+    <row r="133" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B133" s="3"/>
+      <c r="C133" s="3"/>
+      <c r="D133" s="3"/>
+      <c r="E133" s="3"/>
+      <c r="F133" s="3"/>
+      <c r="G133" s="3"/>
+    </row>
+    <row r="134" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B134" s="3"/>
+      <c r="C134" s="3"/>
+      <c r="D134" s="3"/>
+      <c r="E134" s="3"/>
+      <c r="F134" s="3"/>
+      <c r="G134" s="3"/>
+    </row>
+    <row r="135" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B135" s="3"/>
+      <c r="C135" s="3"/>
+      <c r="D135" s="3"/>
+      <c r="E135" s="3"/>
+      <c r="F135" s="3"/>
+      <c r="G135" s="3"/>
+    </row>
+    <row r="136" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B136" s="3"/>
+      <c r="C136" s="3"/>
+      <c r="D136" s="3"/>
+      <c r="E136" s="3"/>
+      <c r="F136" s="3"/>
+      <c r="G136" s="3"/>
+    </row>
+    <row r="137" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B137" s="3"/>
+      <c r="C137" s="3"/>
+      <c r="D137" s="3"/>
+      <c r="E137" s="3"/>
+      <c r="F137" s="3"/>
+      <c r="G137" s="3"/>
+    </row>
+    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B138" s="3"/>
+      <c r="C138" s="3"/>
+      <c r="D138" s="3"/>
+      <c r="E138" s="3"/>
+      <c r="F138" s="3"/>
+      <c r="G138" s="3"/>
+    </row>
+    <row r="139" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B139" s="3"/>
+      <c r="C139" s="3"/>
+      <c r="D139" s="3"/>
+      <c r="E139" s="3"/>
+      <c r="F139" s="3"/>
+      <c r="G139" s="3"/>
+    </row>
+    <row r="140" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B140" s="3"/>
+      <c r="C140" s="3"/>
+      <c r="D140" s="3"/>
+      <c r="E140" s="3"/>
+      <c r="F140" s="3"/>
+      <c r="G140" s="3"/>
+    </row>
+    <row r="141" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B141" s="3"/>
+      <c r="C141" s="3"/>
+      <c r="D141" s="3"/>
+      <c r="E141" s="3"/>
+      <c r="F141" s="3"/>
+      <c r="G141" s="3"/>
+    </row>
+    <row r="142" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B142" s="3"/>
+      <c r="C142" s="3"/>
+      <c r="D142" s="3"/>
+      <c r="E142" s="3"/>
+      <c r="F142" s="3"/>
+      <c r="G142" s="3"/>
+    </row>
+    <row r="143" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B143" s="3"/>
+      <c r="C143" s="3"/>
+      <c r="D143" s="3"/>
+      <c r="E143" s="3"/>
+      <c r="F143" s="3"/>
+      <c r="G143" s="3"/>
+    </row>
+    <row r="144" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B144" s="3"/>
+      <c r="C144" s="3"/>
+      <c r="D144" s="3"/>
+      <c r="E144" s="3"/>
+      <c r="F144" s="3"/>
+      <c r="G144" s="3"/>
+    </row>
+    <row r="145" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B145" s="3"/>
+      <c r="C145" s="3"/>
+      <c r="D145" s="3"/>
+      <c r="E145" s="3"/>
+      <c r="F145" s="3"/>
+      <c r="G145" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Unstable.(haven't checked yet) Feel like little tired of logger. I already can't distinguish what I should log and what not. Probably I added enough logs.
</commit_message>
<xml_diff>
--- a/Blopnote/blopnote bugs and notes.xlsx
+++ b/Blopnote/blopnote bugs and notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azgel\source\repos\Blopnote\Blopnote\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC080D6C-B825-4127-A09A-4D4D737F8165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CA5649-92D6-49E6-BCF9-E27BE850AB5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7D1902E2-70B7-47CB-86DF-C5450FDE41FB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="111">
   <si>
     <t>ID</t>
   </si>
@@ -357,6 +357,12 @@
   </si>
   <si>
     <t>FileProcessor.AskPath() works in awkward way</t>
+  </si>
+  <si>
+    <t>add logs everywhere</t>
+  </si>
+  <si>
+    <t>add webdriver changing</t>
   </si>
 </sst>
 </file>
@@ -788,7 +794,7 @@
   <dimension ref="A1:P145"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A42" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1648,18 +1654,22 @@
       <c r="A46" s="4">
         <v>45</v>
       </c>
-      <c r="B46" s="3"/>
+      <c r="B46" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="13"/>
       <c r="G46" s="3"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>46</v>
       </c>
-      <c r="B47" s="3"/>
+      <c r="B47" s="3" t="s">
+        <v>110</v>
+      </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>

</xml_diff>